<commit_message>
[ttml2] Add editorial tasks assigned to nigel
</commit_message>
<xml_diff>
--- a/ttml2/spec/ednotes.xlsx
+++ b/ttml2/spec/ednotes.xlsx
@@ -1,14 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="16980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$106</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="191">
   <si>
     <t>Section</t>
   </si>
@@ -580,6 +583,18 @@
   </si>
   <si>
     <t>justification in inline progression dimension</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>nigel</t>
+  </si>
+  <si>
+    <t>based on linePadding</t>
+  </si>
+  <si>
+    <t>based on multiRowAlign</t>
   </si>
 </sst>
 </file>
@@ -1248,23 +1263,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="9"/>
     <col min="2" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="63" customWidth="1"/>
+    <col min="3" max="3" width="36.83203125" customWidth="1"/>
     <col min="4" max="5" width="10.83203125" style="7"/>
     <col min="6" max="6" width="10.83203125" style="5"/>
-    <col min="7" max="7" width="76" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>172</v>
       </c>
@@ -1286,8 +1301,11 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1303,8 +1321,11 @@
       <c r="E2" s="7" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1324,7 +1345,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1344,7 +1365,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1364,7 +1385,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1384,7 +1405,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1404,7 +1425,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1424,7 +1445,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1444,7 +1465,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1464,7 +1485,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1481,7 +1502,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1498,7 +1519,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1515,7 +1536,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1532,7 +1553,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1549,7 +1570,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -1856,7 +1877,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -1872,8 +1893,11 @@
       <c r="E33" s="7" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -1890,7 +1914,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -1907,7 +1931,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -1924,7 +1948,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:8">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -1941,7 +1965,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8">
       <c r="A38" s="9">
         <v>37</v>
       </c>
@@ -1961,7 +1985,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -1981,7 +2005,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -1998,7 +2022,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -2018,7 +2042,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:8">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -2038,7 +2062,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:8">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -2055,7 +2079,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -2072,7 +2096,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -2088,8 +2112,11 @@
       <c r="E45" s="7" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="H45" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -2106,7 +2133,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -2126,7 +2153,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:8">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -2146,7 +2173,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:8">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -2166,7 +2193,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:8">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -2183,7 +2210,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:8">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -2199,8 +2226,14 @@
       <c r="E51" s="7" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51" t="s">
+        <v>189</v>
+      </c>
+      <c r="H51" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -2217,7 +2250,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:8">
       <c r="A53" s="9">
         <v>52</v>
       </c>
@@ -2234,7 +2267,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:8">
       <c r="A54" s="9">
         <v>53</v>
       </c>
@@ -2251,7 +2284,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:8">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -2268,7 +2301,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:8">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -2285,7 +2318,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:8">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -2302,7 +2335,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:8">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -2319,7 +2352,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:8">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -2336,7 +2369,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:8">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -2353,7 +2386,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:8">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -2370,7 +2403,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:8">
       <c r="A62" s="9">
         <v>61</v>
       </c>
@@ -2387,7 +2420,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:8">
       <c r="A63" s="9">
         <v>62</v>
       </c>
@@ -2403,8 +2436,14 @@
       <c r="E63" s="7" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63" t="s">
+        <v>190</v>
+      </c>
+      <c r="H63" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="9">
         <v>63</v>
       </c>
@@ -3013,7 +3052,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:8">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -3030,7 +3069,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:8">
       <c r="A98" s="9">
         <v>97</v>
       </c>
@@ -3047,7 +3086,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:8">
       <c r="A99" s="9">
         <v>98</v>
       </c>
@@ -3064,7 +3103,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:8">
       <c r="A100" s="9">
         <v>99</v>
       </c>
@@ -3084,7 +3123,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:8">
       <c r="A101" s="9">
         <v>100</v>
       </c>
@@ -3104,7 +3143,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:8">
       <c r="A102" s="9">
         <v>101</v>
       </c>
@@ -3121,7 +3160,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:8">
       <c r="A103" s="9">
         <v>102</v>
       </c>
@@ -3140,8 +3179,11 @@
       <c r="F103" s="5">
         <v>369</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="H103" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
       <c r="A104" s="9">
         <v>103</v>
       </c>
@@ -3160,8 +3202,11 @@
       <c r="F104" s="5">
         <v>370</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="H104" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105" s="9">
         <v>104</v>
       </c>
@@ -3178,7 +3223,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:8">
       <c r="A106" s="9">
         <v>105</v>
       </c>
@@ -3196,6 +3241,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H106"/>
   <sortState ref="A2:G105">
     <sortCondition ref="A2:A105"/>
   </sortState>

</xml_diff>

<commit_message>
[ttml2] ensure styling references are resolvable
</commit_message>
<xml_diff>
--- a/ttml2/spec/ednotes.xlsx
+++ b/ttml2/spec/ednotes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1250,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1306,133 +1306,127 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="9">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>174</v>
+      <c r="F3" s="5">
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="9">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>165</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>175</v>
+      <c r="F4" s="5">
+        <v>352</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="9">
-        <v>4</v>
+        <v>102</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>180</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>174</v>
+      <c r="F5" s="5">
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="9">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>182</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>174</v>
+      <c r="F6" s="5">
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="9">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>130</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="9">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="9">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>47</v>
@@ -1441,18 +1435,18 @@
         <v>171</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="9">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>178</v>
+        <v>6</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>47</v>
@@ -1461,103 +1455,118 @@
         <v>171</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="9">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="9">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="9">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="9">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="9">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="9">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>133</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
+        <v>178</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>47</v>
@@ -1565,22 +1574,22 @@
       <c r="E16" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="F16" s="5">
-        <v>362</v>
+      <c r="G16" s="10" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="9">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>171</v>
@@ -1588,13 +1597,13 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="9">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>47</v>
@@ -1605,13 +1614,13 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="9">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>47</v>
@@ -1622,13 +1631,13 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="9">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>47</v>
@@ -1639,33 +1648,30 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="9">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>135</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
+        <v>18</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="F21" s="5">
-        <v>333</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="9">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C22" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>47</v>
@@ -1673,39 +1679,36 @@
       <c r="E22" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>139</v>
+      <c r="F22" s="5">
+        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="9">
+        <v>17</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C23" t="s">
-        <v>141</v>
-      </c>
       <c r="D23" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="F23" s="5">
-        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="9">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>47</v>
@@ -1716,13 +1719,13 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="9">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>47</v>
@@ -1733,13 +1736,13 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="9">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C26" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>47</v>
@@ -1748,58 +1751,61 @@
         <v>171</v>
       </c>
       <c r="F26" s="5">
-        <v>302</v>
+        <v>333</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="9">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C27" t="s">
-        <v>185</v>
+        <v>138</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="F27" s="5">
-        <v>380</v>
+      <c r="F27" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="9">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F28" s="5">
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="9">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>171</v>
@@ -1807,16 +1813,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="9">
+        <v>24</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" t="s">
-        <v>35</v>
-      </c>
       <c r="D30" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>171</v>
@@ -1824,19 +1830,22 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="9">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F31" s="5">
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1858,16 +1867,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="9">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>171</v>
@@ -1875,16 +1884,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="9">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>171</v>
@@ -1892,64 +1901,73 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="9">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="G35" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="9">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="G36" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="9">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>50</v>
+        <v>183</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>184</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F37" s="5">
+        <v>379</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="9">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>53</v>
+        <v>144</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>47</v>
@@ -1957,56 +1975,56 @@
       <c r="E38" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="G38" t="s">
-        <v>56</v>
+      <c r="F38" s="5">
+        <v>374</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="9">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="G39" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="9">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="C40" t="s">
-        <v>58</v>
+        <v>146</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F40" s="5">
+        <v>284</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="9">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>183</v>
+        <v>145</v>
       </c>
       <c r="C41" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>47</v>
@@ -2015,18 +2033,18 @@
         <v>171</v>
       </c>
       <c r="F41" s="5">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="9">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>59</v>
+        <v>145</v>
       </c>
       <c r="C42" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>47</v>
@@ -2035,21 +2053,21 @@
         <v>171</v>
       </c>
       <c r="F42" s="5">
-        <v>374</v>
+        <v>379</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="9">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>171</v>
@@ -2057,13 +2075,13 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="9">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>47</v>
@@ -2074,16 +2092,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="9">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C45" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>171</v>
@@ -2091,16 +2109,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="9">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C46" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>171</v>
@@ -2108,93 +2126,87 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="9">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="C47" t="s">
-        <v>146</v>
+        <v>80</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="F47" s="5">
-        <v>284</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="9">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="F48" s="5">
-        <v>373</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="9">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="C49" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="F49" s="5">
-        <v>379</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="9">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>66</v>
+        <v>148</v>
       </c>
       <c r="C50" t="s">
-        <v>67</v>
+        <v>149</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F50" s="5">
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="9">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>171</v>
@@ -2202,16 +2214,16 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="9">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="C52" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>171</v>
@@ -2219,13 +2231,13 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="9">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="C53" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>47</v>
@@ -2236,47 +2248,53 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="9">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>151</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E54" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F54" s="5">
+        <v>365</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="9">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>72</v>
+        <v>152</v>
       </c>
       <c r="C55" t="s">
-        <v>75</v>
+        <v>153</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F55" s="5">
+        <v>324</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="9">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="C56" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>47</v>
@@ -2287,50 +2305,56 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="9">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C57" t="s">
-        <v>78</v>
+        <v>179</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F57" s="5">
+        <v>368</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="9">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="C58" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F58" s="5">
+        <v>147</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="9">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="C59" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>171</v>
@@ -2338,33 +2362,36 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="9">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F60" s="5">
+        <v>338</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="9">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="C61" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E61" s="7" t="s">
         <v>171</v>
@@ -2372,50 +2399,56 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="9">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>85</v>
+        <v>154</v>
       </c>
       <c r="C62" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F62" s="5">
+        <v>293</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="9">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>85</v>
+        <v>156</v>
       </c>
       <c r="C63" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F63" s="5">
+        <v>338</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="9">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>171</v>
@@ -2423,33 +2456,36 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="9">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="C65" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F65" s="5">
+        <v>355</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="9">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="C66" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E66" s="7" t="s">
         <v>171</v>
@@ -2457,30 +2493,33 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="9">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="C67" t="s">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E67" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F67" s="5">
+        <v>358</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="9">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C68" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>47</v>
@@ -2489,52 +2528,58 @@
         <v>171</v>
       </c>
       <c r="F68" s="5">
-        <v>179</v>
+        <v>361</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="9">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>96</v>
+        <v>160</v>
       </c>
       <c r="C69" t="s">
-        <v>97</v>
+        <v>161</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E69" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F69" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="9">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="C70" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E70" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F70" s="5">
+        <v>328</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="9">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="C71" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>47</v>
@@ -2545,13 +2590,13 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="9">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="C72" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>47</v>
@@ -2560,18 +2605,18 @@
         <v>171</v>
       </c>
       <c r="F72" s="5">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="9">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="C73" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>47</v>
@@ -2580,18 +2625,18 @@
         <v>171</v>
       </c>
       <c r="F73" s="5">
-        <v>324</v>
+        <v>351</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="9">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="C74" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>47</v>
@@ -2602,53 +2647,47 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="9">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="C75" t="s">
-        <v>179</v>
+        <v>122</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E75" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="F75" s="5">
-        <v>368</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="9">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="C76" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E76" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="F76" s="5">
-        <v>147</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="9">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="C77" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>47</v>
@@ -2659,50 +2698,50 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="9">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="C78" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E78" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="F78" s="5">
-        <v>338</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="9">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="C79" t="s">
-        <v>106</v>
+        <v>168</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E79" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="F79" s="5">
+        <v>306</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="9">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="C80" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>47</v>
@@ -2711,75 +2750,69 @@
         <v>171</v>
       </c>
       <c r="F80" s="5">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="9">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>156</v>
+        <v>19</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="E81" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="F81" s="5">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" s="9">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>108</v>
+        <v>30</v>
       </c>
       <c r="C82" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="E82" s="7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:5">
       <c r="A83" s="9">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="C83" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="E83" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="F83" s="5">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" s="9">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>110</v>
+        <v>34</v>
       </c>
       <c r="C84" t="s">
-        <v>112</v>
+        <v>35</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>91</v>
@@ -2788,15 +2821,15 @@
         <v>171</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:5">
       <c r="A85" s="9">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>113</v>
+        <v>36</v>
       </c>
       <c r="C85" t="s">
-        <v>114</v>
+        <v>37</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>91</v>
@@ -2805,314 +2838,287 @@
         <v>171</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:5">
       <c r="A86" s="9">
+        <v>51</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C86" t="s">
+        <v>71</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="9">
+        <v>32</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C87" t="s">
+        <v>40</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="9">
+        <v>33</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C88" t="s">
+        <v>42</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="9">
+        <v>36</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C89" t="s">
+        <v>51</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="9">
+        <v>39</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C90" t="s">
+        <v>58</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="9">
+        <v>42</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C91" t="s">
+        <v>60</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="9">
+        <v>44</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C92" t="s">
+        <v>63</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="9">
+        <v>45</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="9">
+        <v>49</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C94" t="s">
+        <v>67</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="9">
+        <v>50</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C95" t="s">
+        <v>69</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="9">
+        <v>56</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C96" t="s">
+        <v>78</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="9">
+        <v>58</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C97" t="s">
+        <v>83</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="9">
+        <v>60</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C98" t="s">
+        <v>84</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="9">
+        <v>62</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C86" t="s">
-        <v>116</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87" s="9">
+      <c r="C99" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C87" t="s">
-        <v>158</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F87" s="5">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="9">
+      <c r="D99" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="9">
+        <v>63</v>
+      </c>
+      <c r="B100" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B88" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C88" t="s">
-        <v>159</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F88" s="5">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="9">
+      <c r="C100" t="s">
         <v>88</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C89" t="s">
-        <v>161</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F89" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" s="9">
+      <c r="D100" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="9">
+        <v>64</v>
+      </c>
+      <c r="B101" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C90" t="s">
-        <v>118</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F90" s="5">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91" s="9">
+      <c r="C101" t="s">
         <v>90</v>
       </c>
-      <c r="B91" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C91" t="s">
-        <v>119</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
-      <c r="A92" s="9">
+      <c r="D101" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B92" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C92" t="s">
-        <v>163</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F92" s="5">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
-      <c r="A93" s="9">
+      <c r="E101" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="9">
+        <v>65</v>
+      </c>
+      <c r="B102" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B93" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C93" t="s">
-        <v>165</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E93" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F93" s="5">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94" s="9">
+      <c r="C102" t="s">
         <v>93</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C94" t="s">
-        <v>166</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E94" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F94" s="5">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="9">
-        <v>94</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C95" t="s">
-        <v>121</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96" s="9">
-        <v>95</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C96" t="s">
-        <v>122</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97" s="9">
-        <v>96</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C97" t="s">
-        <v>123</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="9">
-        <v>97</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C98" t="s">
-        <v>124</v>
-      </c>
-      <c r="D98" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E98" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="9">
-        <v>98</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C99" t="s">
-        <v>126</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="9">
-        <v>99</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C100" t="s">
-        <v>168</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E100" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F100" s="5">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101" s="9">
-        <v>100</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C101" t="s">
-        <v>170</v>
-      </c>
-      <c r="D101" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E101" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F101" s="5">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
-      <c r="A102" s="9">
-        <v>101</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C102" t="s">
-        <v>128</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>91</v>
@@ -3121,83 +3127,77 @@
         <v>171</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:5">
       <c r="A103" s="9">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>180</v>
+        <v>94</v>
       </c>
       <c r="C103" t="s">
-        <v>181</v>
+        <v>95</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="F103" s="5">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" s="9">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>180</v>
+        <v>110</v>
       </c>
       <c r="C104" t="s">
-        <v>182</v>
+        <v>112</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="E104" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="F104" s="5">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" s="9">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C105" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="E105" s="7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:5">
       <c r="A106" s="9">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C106" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="E106" s="7" t="s">
         <v>171</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G105">
-    <sortCondition ref="A2:A105"/>
+  <sortState ref="A2:G106">
+    <sortCondition ref="D2:D106"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
[ttml2] Add Pierre to ednotes spreadsheet for disparity example
</commit_message>
<xml_diff>
--- a/ttml2/spec/ednotes.xlsx
+++ b/ttml2/spec/ednotes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="192">
   <si>
     <t>Section</t>
   </si>
@@ -595,6 +595,9 @@
   </si>
   <si>
     <t>based on multiRowAlign</t>
+  </si>
+  <si>
+    <t>pierre</t>
   </si>
 </sst>
 </file>
@@ -1265,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="H105" sqref="H105"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1913,6 +1916,9 @@
       <c r="E34" s="7" t="s">
         <v>171</v>
       </c>
+      <c r="H34" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="9">

</xml_diff>

<commit_message>
[ttml2] Mark editorial actions 001, 102 and 103 as C.
</commit_message>
<xml_diff>
--- a/ttml2/spec/ednotes.xlsx
+++ b/ttml2/spec/ednotes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="800" yWindow="12120" windowWidth="18060" windowHeight="16980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="193">
   <si>
     <t>Section</t>
   </si>
@@ -598,6 +598,9 @@
   </si>
   <si>
     <t>pierre</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -1268,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1322,7 +1325,7 @@
         <v>48</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="H2" t="s">
         <v>188</v>
@@ -3180,7 +3183,7 @@
         <v>48</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="F103" s="5">
         <v>369</v>
@@ -3203,7 +3206,7 @@
         <v>48</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="F104" s="5">
         <v>370</v>

</xml_diff>

<commit_message>
[ttml] Address editorial note for padding on content element example.
Added second padding example document fragment.
Added padding_2.png example and padding_2.html source (png generated by manually cropping screenshot of rendered html).
Updated ednotes.xlsx to indicate that this editorial note is closed.
</commit_message>
<xml_diff>
--- a/ttml2/spec/ednotes.xlsx
+++ b/ttml2/spec/ednotes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="12120" windowWidth="18060" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="8820" yWindow="1980" windowWidth="18060" windowHeight="16980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1269,10 +1269,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1311,7 +1312,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" hidden="1">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1331,7 +1332,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1351,7 +1352,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1371,7 +1372,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" hidden="1">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1391,7 +1392,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1411,7 +1412,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" hidden="1">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1431,7 +1432,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1451,7 +1452,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1471,7 +1472,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1491,7 +1492,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" hidden="1">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" hidden="1">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1525,7 +1526,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1542,7 +1543,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" hidden="1">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1559,7 +1560,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1576,7 +1577,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" hidden="1">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" hidden="1">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -1613,7 +1614,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" hidden="1">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" hidden="1">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -1647,7 +1648,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" hidden="1">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -1664,7 +1665,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" hidden="1">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -1684,7 +1685,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" hidden="1">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -1704,7 +1705,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" hidden="1">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -1724,7 +1725,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" hidden="1">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -1741,7 +1742,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" hidden="1">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -1758,7 +1759,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" hidden="1">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -1778,7 +1779,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" hidden="1">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" hidden="1">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -1815,7 +1816,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" hidden="1">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -1832,7 +1833,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" hidden="1">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -1849,7 +1850,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" hidden="1">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" hidden="1">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -1903,7 +1904,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" hidden="1">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -1923,7 +1924,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" hidden="1">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -1940,7 +1941,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" hidden="1">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -1957,7 +1958,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" hidden="1">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -1974,7 +1975,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" hidden="1">
       <c r="A38" s="9">
         <v>37</v>
       </c>
@@ -1994,7 +1995,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" hidden="1">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -2014,7 +2015,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" hidden="1">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -2031,7 +2032,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" hidden="1">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -2051,7 +2052,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" hidden="1">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -2071,7 +2072,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" hidden="1">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -2088,7 +2089,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" hidden="1">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" hidden="1">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -2142,7 +2143,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" hidden="1">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -2162,7 +2163,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" hidden="1">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -2182,7 +2183,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" hidden="1">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -2202,7 +2203,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" hidden="1">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -2233,7 +2234,7 @@
         <v>91</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="G51" t="s">
         <v>189</v>
@@ -2242,7 +2243,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" hidden="1">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -2259,7 +2260,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" hidden="1">
       <c r="A53" s="9">
         <v>52</v>
       </c>
@@ -2276,7 +2277,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" hidden="1">
       <c r="A54" s="9">
         <v>53</v>
       </c>
@@ -2293,7 +2294,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" hidden="1">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -2310,7 +2311,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" hidden="1">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -2327,7 +2328,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" hidden="1">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" hidden="1">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -2361,7 +2362,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" hidden="1">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -2378,7 +2379,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" hidden="1">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -2395,7 +2396,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" hidden="1">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" hidden="1">
       <c r="A62" s="9">
         <v>61</v>
       </c>
@@ -2452,7 +2453,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" hidden="1">
       <c r="A64" s="9">
         <v>63</v>
       </c>
@@ -2469,7 +2470,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" hidden="1">
       <c r="A65" s="9">
         <v>64</v>
       </c>
@@ -2486,7 +2487,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" hidden="1">
       <c r="A66" s="9">
         <v>65</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" hidden="1">
       <c r="A67" s="9">
         <v>66</v>
       </c>
@@ -2520,7 +2521,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" hidden="1">
       <c r="A68" s="9">
         <v>67</v>
       </c>
@@ -2540,7 +2541,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" hidden="1">
       <c r="A69" s="9">
         <v>68</v>
       </c>
@@ -2557,7 +2558,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" hidden="1">
       <c r="A70" s="9">
         <v>69</v>
       </c>
@@ -2574,7 +2575,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" hidden="1">
       <c r="A71" s="9">
         <v>70</v>
       </c>
@@ -2591,7 +2592,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" hidden="1">
       <c r="A72" s="9">
         <v>71</v>
       </c>
@@ -2611,7 +2612,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" hidden="1">
       <c r="A73" s="9">
         <v>72</v>
       </c>
@@ -2631,7 +2632,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" hidden="1">
       <c r="A74" s="9">
         <v>73</v>
       </c>
@@ -2648,7 +2649,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" hidden="1">
       <c r="A75" s="9">
         <v>74</v>
       </c>
@@ -2668,7 +2669,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" hidden="1">
       <c r="A76" s="9">
         <v>75</v>
       </c>
@@ -2688,7 +2689,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" hidden="1">
       <c r="A77" s="9">
         <v>76</v>
       </c>
@@ -2705,7 +2706,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" hidden="1">
       <c r="A78" s="9">
         <v>77</v>
       </c>
@@ -2725,7 +2726,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" hidden="1">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -2742,7 +2743,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" hidden="1">
       <c r="A80" s="9">
         <v>79</v>
       </c>
@@ -2762,7 +2763,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" hidden="1">
       <c r="A81" s="9">
         <v>80</v>
       </c>
@@ -2782,7 +2783,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" hidden="1">
       <c r="A82" s="9">
         <v>81</v>
       </c>
@@ -2799,7 +2800,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" hidden="1">
       <c r="A83" s="9">
         <v>82</v>
       </c>
@@ -2819,7 +2820,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" hidden="1">
       <c r="A84" s="9">
         <v>83</v>
       </c>
@@ -2836,7 +2837,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" hidden="1">
       <c r="A85" s="9">
         <v>84</v>
       </c>
@@ -2853,7 +2854,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" hidden="1">
       <c r="A86" s="9">
         <v>85</v>
       </c>
@@ -2870,7 +2871,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" hidden="1">
       <c r="A87" s="9">
         <v>86</v>
       </c>
@@ -2890,7 +2891,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" hidden="1">
       <c r="A88" s="9">
         <v>87</v>
       </c>
@@ -2910,7 +2911,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" hidden="1">
       <c r="A89" s="9">
         <v>88</v>
       </c>
@@ -2930,7 +2931,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" hidden="1">
       <c r="A90" s="9">
         <v>89</v>
       </c>
@@ -2950,7 +2951,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" hidden="1">
       <c r="A91" s="9">
         <v>90</v>
       </c>
@@ -2967,7 +2968,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" hidden="1">
       <c r="A92" s="9">
         <v>91</v>
       </c>
@@ -2987,7 +2988,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" hidden="1">
       <c r="A93" s="9">
         <v>92</v>
       </c>
@@ -3007,7 +3008,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" hidden="1">
       <c r="A94" s="9">
         <v>93</v>
       </c>
@@ -3027,7 +3028,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" hidden="1">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -3044,7 +3045,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" hidden="1">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -3061,7 +3062,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" hidden="1">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -3078,7 +3079,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" hidden="1">
       <c r="A98" s="9">
         <v>97</v>
       </c>
@@ -3095,7 +3096,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" hidden="1">
       <c r="A99" s="9">
         <v>98</v>
       </c>
@@ -3112,7 +3113,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" hidden="1">
       <c r="A100" s="9">
         <v>99</v>
       </c>
@@ -3132,7 +3133,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" hidden="1">
       <c r="A101" s="9">
         <v>100</v>
       </c>
@@ -3152,7 +3153,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" hidden="1">
       <c r="A102" s="9">
         <v>101</v>
       </c>
@@ -3169,7 +3170,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" hidden="1">
       <c r="A103" s="9">
         <v>102</v>
       </c>
@@ -3192,7 +3193,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" hidden="1">
       <c r="A104" s="9">
         <v>103</v>
       </c>
@@ -3215,7 +3216,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" hidden="1">
       <c r="A105" s="9">
         <v>104</v>
       </c>
@@ -3232,7 +3233,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" hidden="1">
       <c r="A106" s="9">
         <v>105</v>
       </c>
@@ -3250,7 +3251,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H106"/>
+  <autoFilter ref="A1:H106">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="O"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="nigel"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:G105">
     <sortCondition ref="A2:A105"/>
   </sortState>

</xml_diff>

<commit_message>
[ttml] Address editorial note: add example for textAlign applied to span
Update ednotes.xlsx
In ttml2.xml remove editorial note, add example fragment and image.
Add textAlign_2.png image, derived by taking screenshot of rendered textAlign_2.html
</commit_message>
<xml_diff>
--- a/ttml2/spec/ednotes.xlsx
+++ b/ttml2/spec/ednotes.xlsx
@@ -1273,7 +1273,7 @@
   <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1332,7 +1332,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" spans="1:8">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" spans="1:8">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" spans="1:8">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1">
+    <row r="17" spans="1:6">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1">
+    <row r="18" spans="1:6">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1">
+    <row r="19" spans="1:6">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1">
+    <row r="20" spans="1:6">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1">
+    <row r="21" spans="1:6">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1">
+    <row r="22" spans="1:6">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1">
+    <row r="23" spans="1:6">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1">
+    <row r="24" spans="1:6">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1">
+    <row r="25" spans="1:6">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1">
+    <row r="26" spans="1:6">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1">
+    <row r="27" spans="1:6">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1">
+    <row r="28" spans="1:6">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1">
+    <row r="29" spans="1:6">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1">
+    <row r="30" spans="1:6">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1">
+    <row r="31" spans="1:6">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1">
+    <row r="32" spans="1:6">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1">
+    <row r="34" spans="1:8">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1">
+    <row r="35" spans="1:8">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1">
+    <row r="36" spans="1:8">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1">
+    <row r="37" spans="1:8">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1">
+    <row r="38" spans="1:8">
       <c r="A38" s="9">
         <v>37</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1">
+    <row r="39" spans="1:8">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1">
+    <row r="40" spans="1:8">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1">
+    <row r="41" spans="1:8">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1">
+    <row r="42" spans="1:8">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1">
+    <row r="43" spans="1:8">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1">
+    <row r="44" spans="1:8">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1">
+    <row r="46" spans="1:8">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1">
+    <row r="47" spans="1:8">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1">
+    <row r="48" spans="1:8">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1">
+    <row r="49" spans="1:8">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1">
+    <row r="50" spans="1:8">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" hidden="1">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1">
+    <row r="52" spans="1:8">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1">
+    <row r="53" spans="1:8">
       <c r="A53" s="9">
         <v>52</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1">
+    <row r="54" spans="1:8">
       <c r="A54" s="9">
         <v>53</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1">
+    <row r="55" spans="1:8">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1">
+    <row r="56" spans="1:8">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1">
+    <row r="57" spans="1:8">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1">
+    <row r="58" spans="1:8">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1">
+    <row r="59" spans="1:8">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1">
+    <row r="60" spans="1:8">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1">
+    <row r="61" spans="1:8">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1">
+    <row r="62" spans="1:8">
       <c r="A62" s="9">
         <v>61</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" hidden="1">
       <c r="A63" s="9">
         <v>62</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>91</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="G63" t="s">
         <v>190</v>
@@ -2453,7 +2453,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1">
+    <row r="64" spans="1:8">
       <c r="A64" s="9">
         <v>63</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1">
+    <row r="65" spans="1:6">
       <c r="A65" s="9">
         <v>64</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1">
+    <row r="66" spans="1:6">
       <c r="A66" s="9">
         <v>65</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1">
+    <row r="67" spans="1:6">
       <c r="A67" s="9">
         <v>66</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1">
+    <row r="68" spans="1:6">
       <c r="A68" s="9">
         <v>67</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1">
+    <row r="69" spans="1:6">
       <c r="A69" s="9">
         <v>68</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1">
+    <row r="70" spans="1:6">
       <c r="A70" s="9">
         <v>69</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1">
+    <row r="71" spans="1:6">
       <c r="A71" s="9">
         <v>70</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1">
+    <row r="72" spans="1:6">
       <c r="A72" s="9">
         <v>71</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1">
+    <row r="73" spans="1:6">
       <c r="A73" s="9">
         <v>72</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1">
+    <row r="74" spans="1:6">
       <c r="A74" s="9">
         <v>73</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1">
+    <row r="75" spans="1:6">
       <c r="A75" s="9">
         <v>74</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1">
+    <row r="76" spans="1:6">
       <c r="A76" s="9">
         <v>75</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1">
+    <row r="77" spans="1:6">
       <c r="A77" s="9">
         <v>76</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1">
+    <row r="78" spans="1:6">
       <c r="A78" s="9">
         <v>77</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1">
+    <row r="79" spans="1:6">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1">
+    <row r="80" spans="1:6">
       <c r="A80" s="9">
         <v>79</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1">
+    <row r="81" spans="1:6">
       <c r="A81" s="9">
         <v>80</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1">
+    <row r="82" spans="1:6">
       <c r="A82" s="9">
         <v>81</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1">
+    <row r="83" spans="1:6">
       <c r="A83" s="9">
         <v>82</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1">
+    <row r="84" spans="1:6">
       <c r="A84" s="9">
         <v>83</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1">
+    <row r="85" spans="1:6">
       <c r="A85" s="9">
         <v>84</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1">
+    <row r="86" spans="1:6">
       <c r="A86" s="9">
         <v>85</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1">
+    <row r="87" spans="1:6">
       <c r="A87" s="9">
         <v>86</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1">
+    <row r="88" spans="1:6">
       <c r="A88" s="9">
         <v>87</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1">
+    <row r="89" spans="1:6">
       <c r="A89" s="9">
         <v>88</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1">
+    <row r="90" spans="1:6">
       <c r="A90" s="9">
         <v>89</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1">
+    <row r="91" spans="1:6">
       <c r="A91" s="9">
         <v>90</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1">
+    <row r="92" spans="1:6">
       <c r="A92" s="9">
         <v>91</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1">
+    <row r="93" spans="1:6">
       <c r="A93" s="9">
         <v>92</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1">
+    <row r="94" spans="1:6">
       <c r="A94" s="9">
         <v>93</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1">
+    <row r="95" spans="1:6">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1">
+    <row r="96" spans="1:6">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1">
+    <row r="97" spans="1:8">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1">
+    <row r="98" spans="1:8">
       <c r="A98" s="9">
         <v>97</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1">
+    <row r="99" spans="1:8">
       <c r="A99" s="9">
         <v>98</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1">
+    <row r="100" spans="1:8">
       <c r="A100" s="9">
         <v>99</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1">
+    <row r="101" spans="1:8">
       <c r="A101" s="9">
         <v>100</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1">
+    <row r="102" spans="1:8">
       <c r="A102" s="9">
         <v>101</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1">
+    <row r="105" spans="1:8">
       <c r="A105" s="9">
         <v>104</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1">
+    <row r="106" spans="1:8">
       <c r="A106" s="9">
         <v>105</v>
       </c>
@@ -3255,11 +3255,6 @@
     <filterColumn colId="4">
       <filters>
         <filter val="O"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters>
-        <filter val="nigel"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>